<commit_message>
update of Starter Code
</commit_message>
<xml_diff>
--- a/Resources/nsclc_tcga_broad_2016_clinical_data.xlsx
+++ b/Resources/nsclc_tcga_broad_2016_clinical_data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adriandelacruz/Desktop/github/Project-4-Predictors-of-Lung-Cancer/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7936B50F-26AE-374E-9E39-DA46C81D8C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA46D8E7-D520-2B44-A27D-C74E021ED5DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34620" yWindow="2180" windowWidth="31060" windowHeight="19540" xr2:uid="{4DBE7499-EB20-3D48-AB69-EE9661ED14E8}"/>
+    <workbookView xWindow="36440" yWindow="5100" windowWidth="27240" windowHeight="16440" xr2:uid="{40B7D5D2-A2D4-D14B-AC70-77D8DD230D4B}"/>
   </bookViews>
   <sheets>
     <sheet name="nsclc_tcga_broad_2016_clinical_" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">nsclc_tcga_broad_2016_clinical_!$A$1:$Z$1145</definedName>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21226" uniqueCount="2366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21296" uniqueCount="2370">
   <si>
     <t>Study ID</t>
   </si>
@@ -7121,7 +7122,19 @@
     <t>Columns dropped</t>
   </si>
   <si>
-    <t>Common value</t>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Single Value?</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>If Y, Value?</t>
+  </si>
+  <si>
+    <t>Columns to be dropped</t>
   </si>
 </sst>
 </file>
@@ -7264,7 +7277,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7444,6 +7457,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -7605,8 +7624,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -7965,7 +7992,7 @@
   <dimension ref="A1:Z1145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -99606,24 +99633,341 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D511DF11-1204-A347-97AC-C7170CD39C77}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>2364</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2366</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2368</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2365</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2367</v>
+      </c>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2367</v>
+      </c>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2367</v>
+      </c>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2367</v>
+      </c>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>2365</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2367</v>
+      </c>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2367</v>
+      </c>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2367</v>
+      </c>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2367</v>
+      </c>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2367</v>
+      </c>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2367</v>
+      </c>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2367</v>
+      </c>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2367</v>
+      </c>
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2367</v>
+      </c>
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2367</v>
+      </c>
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2367</v>
+      </c>
+      <c r="C18" s="4"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2367</v>
+      </c>
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>2365</v>
+      </c>
+      <c r="C20" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>2367</v>
+      </c>
+      <c r="C21" s="4"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2367</v>
+      </c>
+      <c r="C22" s="4"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>2367</v>
+      </c>
+      <c r="C23" s="4"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>2365</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2367</v>
+      </c>
+      <c r="C25" s="4"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>2367</v>
+      </c>
+      <c r="C26" s="4"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2367</v>
+      </c>
+      <c r="C27" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC673058-A636-264A-8BDD-5344068CE513}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>2364</v>
+        <v>2369</v>
       </c>
       <c r="B1" t="s">
+        <v>2366</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2368</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2365</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2365</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2365</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2365</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>